<commit_message>
Added supporting of Liza's computer
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -56,7 +57,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -72,9 +73,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -119,7 +120,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -157,6 +158,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3102-4FBA-89C3-FBD33D833C4E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -183,6 +189,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3102-4FBA-89C3-FBD33D833C4E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -236,7 +247,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="156802312"/>
@@ -295,7 +306,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="156801920"/>
@@ -338,7 +349,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -368,7 +379,314 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$A$1:$A$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="150"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F5FE-4FE3-8345-76EA5523313F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$1:$B$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="150"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F5FE-4FE3-8345-76EA5523313F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="352241984"/>
+        <c:axId val="352238376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="352241984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352238376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="352238376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352241984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -419,6 +737,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -935,20 +1293,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>138112</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -967,13 +1828,43 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1011,7 +1902,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1083,7 +1974,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1260,7 +2151,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,4 +2177,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new generators. Update user interface
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,7 +56,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -73,9 +72,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -120,7 +119,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -158,11 +157,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3102-4FBA-89C3-FBD33D833C4E}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -189,11 +183,6 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3102-4FBA-89C3-FBD33D833C4E}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -204,11 +193,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="156801920"/>
-        <c:axId val="156802312"/>
+        <c:axId val="114205384"/>
+        <c:axId val="114204992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="156801920"/>
+        <c:axId val="114205384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -247,10 +236,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156802312"/>
+        <c:crossAx val="114204992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -258,7 +247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156802312"/>
+        <c:axId val="114204992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -306,10 +295,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156801920"/>
+        <c:crossAx val="114205384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -349,7 +338,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -379,314 +368,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$A$1:$A$150</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F5FE-4FE3-8345-76EA5523313F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$B$1:$B$150</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F5FE-4FE3-8345-76EA5523313F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="352241984"/>
-        <c:axId val="352238376"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="352241984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="352238376"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="352238376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="352241984"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -737,46 +419,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -940,509 +582,6 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1801,15 +940,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1828,43 +967,13 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1902,7 +1011,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1974,7 +1083,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2151,7 +1260,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,16 +1286,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>